<commit_message>
Finish FCR search rankings evaluation
</commit_message>
<xml_diff>
--- a/Formula Concept Retrieval/diff_eqns_examples/ten examples/diff_eqns.xlsx
+++ b/Formula Concept Retrieval/diff_eqns_examples/ten examples/diff_eqns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Meine Ablage (philippscharpfresearch@gmail.com)\PhD\Projects\Formula Concepts\formula-concept-retrieval\Formula Concept Retrieval\diff_eqns_examples\ten examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AAB471-C13D-4932-B5B4-3AEEDCFBC961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E2B823-B147-4405-9D6C-53AA903F4DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="156">
   <si>
     <t xml:space="preserve">Schroedinger equation </t>
   </si>
@@ -60,9 +60,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Equation</t>
-  </si>
-  <si>
     <t>QID</t>
   </si>
   <si>
@@ -493,6 +490,24 @@
   </si>
   <si>
     <t>ME</t>
+  </si>
+  <si>
+    <t>Ex. Equation</t>
+  </si>
+  <si>
+    <t>\frac{1}{c^2} \frac{\partial^2 \psi}{\partial t^2} - \nabla^2 \psi + \left( \frac{m_0 c}{\hbar} \right)^2 \psi = 0</t>
+  </si>
+  <si>
+    <t>G_{\mu \nu} + \Lambda g_{\mu \nu} = \kappa T_{\mu \nu}</t>
+  </si>
+  <si>
+    <t>\text{div} \vec{E} = 4 \pi \rho</t>
+  </si>
+  <si>
+    <t>(\nabla^2 − k^2) A = -f</t>
+  </si>
+  <si>
+    <t>|F_1| = |F_2| = \\frac{|q_1 \\times q_2|}{r^2}</t>
   </si>
 </sst>
 </file>
@@ -1335,29 +1350,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -1365,13 +1380,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -1379,13 +1397,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -1393,13 +1414,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -1407,13 +1431,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -1421,13 +1448,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -1435,80 +1465,95 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>128</v>
       </c>
-      <c r="C7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
         <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
         <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
         <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" t="s">
         <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1522,29 +1567,29 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1552,10 +1597,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -1564,10 +1609,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -1576,10 +1621,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -1588,10 +1633,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -1600,10 +1645,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -1612,10 +1657,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -1624,10 +1669,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -1636,10 +1681,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -1648,10 +1693,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -1660,23 +1705,23 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1696,22 +1741,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1719,10 +1764,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -1731,10 +1776,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -1743,10 +1788,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -1755,10 +1800,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -1767,10 +1812,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -1779,10 +1824,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -1791,10 +1836,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -1803,10 +1848,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -1815,10 +1860,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -1827,31 +1872,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1871,22 +1916,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1894,10 +1939,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -1906,10 +1951,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -1918,10 +1963,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -1930,10 +1975,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -1942,10 +1987,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -1954,10 +1999,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -1966,10 +2011,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -1978,10 +2023,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -1990,10 +2035,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -2002,39 +2047,39 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" t="s">
         <v>142</v>
-      </c>
-      <c r="B14" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" t="s">
         <v>144</v>
-      </c>
-      <c r="B15" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2054,22 +2099,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -2077,10 +2122,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -2089,10 +2134,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -2101,10 +2146,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -2113,10 +2158,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -2125,10 +2170,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -2137,10 +2182,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -2149,10 +2194,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -2161,10 +2206,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -2173,10 +2218,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -2185,23 +2230,23 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2221,22 +2266,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -2244,10 +2289,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -2256,10 +2301,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -2268,10 +2313,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -2280,10 +2325,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -2292,10 +2337,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -2304,10 +2349,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -2316,10 +2361,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -2328,10 +2373,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -2340,10 +2385,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -2352,39 +2397,39 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
         <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2407,22 +2452,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -2430,10 +2475,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -2442,10 +2487,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -2454,10 +2499,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -2466,10 +2511,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -2478,10 +2523,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -2490,10 +2535,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -2502,10 +2547,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -2514,10 +2559,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -2526,10 +2571,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -2538,39 +2583,39 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2595,22 +2640,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -2618,10 +2663,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -2630,10 +2675,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -2642,10 +2687,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -2654,10 +2699,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -2666,10 +2711,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -2678,10 +2723,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -2690,10 +2735,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -2702,10 +2747,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -2714,10 +2759,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -2726,23 +2771,23 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2765,22 +2810,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -2788,10 +2833,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -2800,10 +2845,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
@@ -2812,10 +2857,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
@@ -2824,10 +2869,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -2836,10 +2881,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -2848,10 +2893,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -2860,10 +2905,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -2872,10 +2917,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -2884,10 +2929,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -2896,23 +2941,23 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>